<commit_message>
completed - rectified errors
completed - rectified errors
</commit_message>
<xml_diff>
--- a/1. Statistics and Machine Learning/4. Investment Assignment/Investments.xlsx
+++ b/1. Statistics and Machine Learning/4. Investment Assignment/Investments.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187">
   <si>
     <t>Table-1.1</t>
   </si>
@@ -339,153 +339,159 @@
     <t>Third English speaking country</t>
   </si>
   <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>Table - 5.1</t>
+  </si>
+  <si>
+    <t>Sector-wise Investment Analysis</t>
+  </si>
+  <si>
+    <t>Sl.no</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Total number of Investments (count)</t>
+  </si>
+  <si>
+    <t>Total amount of investment (USD)</t>
+  </si>
+  <si>
+    <t>Top Sector name (no. of investment-wise)</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Second Sector name (no. of investment-wise)</t>
+  </si>
+  <si>
+    <t>Social, Finance, Analytics, Advertising</t>
+  </si>
+  <si>
+    <t>Third Sector name (no. of investment-wise)</t>
+  </si>
+  <si>
+    <t>Cleantech / Semiconductors</t>
+  </si>
+  <si>
+    <t>News, Search and Messaging</t>
+  </si>
+  <si>
+    <t>Number of investments in top sector (3)</t>
+  </si>
+  <si>
+    <t>Number of investments in second sector (4)</t>
+  </si>
+  <si>
+    <t>Number of investments in third sector (5)</t>
+  </si>
+  <si>
+    <t>For point 3 (top sector count-wise), which company received the highest investment?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/organization/virtustream </t>
+  </si>
+  <si>
+    <t>/organization/electric-cloud</t>
+  </si>
+  <si>
+    <t>/organization/firstcry-com</t>
+  </si>
+  <si>
+    <t>For point 4 (second best sector count-wise), which company received the highest investment?</t>
+  </si>
+  <si>
+    <t>/organization/shotspotter</t>
+  </si>
+  <si>
+    <t>/organization/celltick-technologies</t>
+  </si>
+  <si>
+    <t>/organization/manthan-systems</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Country code</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Caribbean</t>
+  </si>
+  <si>
+    <t>ATG</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
+    <t>Bahamas, The</t>
+  </si>
+  <si>
+    <t>BHS</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>BRB</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Central America / Caribbean</t>
+  </si>
+  <si>
+    <t>BLZ</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>BWA</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>CMR</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
     <t>CAN</t>
   </si>
   <si>
-    <t>Table - 5.1</t>
-  </si>
-  <si>
-    <t>Sector-wise Investment Analysis</t>
-  </si>
-  <si>
-    <t>Sl.no</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>Total number of Investments (count)</t>
-  </si>
-  <si>
-    <t>Total amount of investment (USD)</t>
-  </si>
-  <si>
-    <t>Top Sector name (no. of investment-wise)</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>Cleantech / Semiconductors</t>
-  </si>
-  <si>
-    <t>Second Sector name (no. of investment-wise)</t>
-  </si>
-  <si>
-    <t>Social, Finance, Analytics, Advertising</t>
-  </si>
-  <si>
-    <t>Third Sector name (no. of investment-wise)</t>
-  </si>
-  <si>
-    <t>Number of investments in top sector (3)</t>
-  </si>
-  <si>
-    <t>Number of investments in second sector (4)</t>
-  </si>
-  <si>
-    <t>Number of investments in third sector (5)</t>
-  </si>
-  <si>
-    <t>For point 3 (top sector count-wise), which company received the highest investment?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/organization/virtustream </t>
-  </si>
-  <si>
-    <t>/organization/electric-cloud</t>
-  </si>
-  <si>
-    <t>/organization/fresco-microchip</t>
-  </si>
-  <si>
-    <t>For point 4 (second best sector count-wise), which company received the highest investment?</t>
-  </si>
-  <si>
-    <t>/organization/shotspotter</t>
-  </si>
-  <si>
-    <t>/organization/celltick-technologies</t>
-  </si>
-  <si>
-    <t>/organization/quickplay-media</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Population</t>
-  </si>
-  <si>
-    <t>Country code</t>
-  </si>
-  <si>
-    <t>Antigua and Barbuda</t>
-  </si>
-  <si>
-    <t>Caribbean</t>
-  </si>
-  <si>
-    <t>ATG</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>AUS</t>
-  </si>
-  <si>
-    <t>Bahamas, The</t>
-  </si>
-  <si>
-    <t>BHS</t>
-  </si>
-  <si>
-    <t>Barbados</t>
-  </si>
-  <si>
-    <t>BRB</t>
-  </si>
-  <si>
-    <t>Belize</t>
-  </si>
-  <si>
-    <t>Central America / Caribbean</t>
-  </si>
-  <si>
-    <t>BLZ</t>
-  </si>
-  <si>
-    <t>Botswana</t>
-  </si>
-  <si>
-    <t>Africa</t>
-  </si>
-  <si>
-    <t>BWA</t>
-  </si>
-  <si>
-    <t>Cameroon</t>
-  </si>
-  <si>
-    <t>CMR</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>North America</t>
-  </si>
-  <si>
     <t>Dominica</t>
   </si>
   <si>
@@ -544,9 +550,6 @@
   </si>
   <si>
     <t>Asia</t>
-  </si>
-  <si>
-    <t>IND</t>
   </si>
   <si>
     <t>Ireland</t>
@@ -815,8 +818,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -882,17 +885,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -904,54 +920,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -966,25 +937,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -996,15 +952,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1017,9 +1014,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1067,7 +1070,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,13 +1142,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1103,7 +1166,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1115,13 +1208,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1133,55 +1226,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1193,55 +1244,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1376,6 +1379,41 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1386,21 +1424,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1428,175 +1451,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1701,9 +1704,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2075,7 +2075,7 @@
       <c r="A5" s="36">
         <v>1</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="16">
@@ -2086,7 +2086,7 @@
       <c r="A6" s="36">
         <v>2</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="16">
@@ -2097,7 +2097,7 @@
       <c r="A7" s="36">
         <v>3</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -2108,7 +2108,7 @@
       <c r="A8" s="36">
         <v>4</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="16" t="s">
@@ -2119,7 +2119,7 @@
       <c r="A9" s="36">
         <v>5</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="16">
@@ -2127,10 +2127,10 @@
       </c>
     </row>
     <row r="10" spans="2:2">
-      <c r="B10" s="39"/>
+      <c r="B10" s="38"/>
     </row>
     <row r="11" spans="2:2">
-      <c r="B11" s="39"/>
+      <c r="B11" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2278,7 +2278,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -2375,7 +2375,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2437,7 +2437,7 @@
         <v>621</v>
       </c>
       <c r="E5" s="16">
-        <v>422</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2454,10 +2454,10 @@
         <v>5379078691</v>
       </c>
       <c r="E6" s="16">
-        <v>3599289960</v>
-      </c>
-    </row>
-    <row r="7" ht="30" spans="1:5">
+        <v>2949543602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="14">
         <v>3</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>39</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" ht="45" spans="1:5">
@@ -2479,33 +2479,33 @@
         <v>4</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>42</v>
-      </c>
       <c r="D8" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" ht="45" spans="1:5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" ht="30" spans="1:5">
       <c r="A9" s="14">
         <v>5</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>40</v>
-      </c>
       <c r="D9" s="17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2513,7 +2513,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="16">
         <v>2950</v>
@@ -2522,7 +2522,7 @@
         <v>147</v>
       </c>
       <c r="E10" s="16">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2530,7 +2530,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="16">
         <v>2714</v>
@@ -2539,7 +2539,7 @@
         <v>133</v>
       </c>
       <c r="E11" s="16">
-        <v>109</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2547,7 +2547,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="16">
         <v>2350</v>
@@ -2556,7 +2556,7 @@
         <v>130</v>
       </c>
       <c r="E12" s="16">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" ht="30" spans="1:5">
@@ -2564,16 +2564,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" ht="45.75" spans="1:5">
@@ -2581,16 +2581,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2662,782 +2662,782 @@
     <col min="3" max="4" width="13.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:4">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" ht="45" spans="1:4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3">
         <v>85000</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" s="3">
         <v>22374370</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" ht="30" spans="1:4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3">
         <v>331000</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" ht="30" spans="1:4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3">
         <v>294000</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" ht="75" spans="1:4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" ht="30" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C6" s="3">
         <v>288000</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" ht="30" spans="1:4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3">
         <v>1882000</v>
       </c>
       <c r="D7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="8" ht="30" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C8" s="3">
         <v>18549000</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" ht="30" spans="1:4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3">
         <v>33531000</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" ht="30" spans="1:4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3">
         <v>73000</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" s="3">
         <v>5224000</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C12" s="3">
         <v>82101998</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C13" s="3">
         <v>827900</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" ht="30" spans="1:4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C14" s="3">
         <v>1709000</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C15" s="3">
         <v>23478000</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" ht="30" spans="1:4">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" s="3">
         <v>106000</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" ht="75" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" ht="30" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C17" s="3">
         <v>738000</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C18" s="3">
         <v>1143540000</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C19" s="3">
         <v>4581269</v>
       </c>
       <c r="D19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" ht="30" spans="1:4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C20" s="3">
         <v>2714000</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C21" s="3">
         <v>37538000</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C22" s="3">
         <v>95000</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" ht="60" spans="1:4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" ht="30" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C23" s="3">
         <v>17000000</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C24" s="3">
         <v>2008000</v>
       </c>
       <c r="D24" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" s="3">
         <v>3750000</v>
       </c>
       <c r="D25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C26" s="3">
         <v>13925000</v>
       </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C27" s="3">
         <v>412600</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" ht="30" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C28" s="3">
         <v>59000</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" ht="45" spans="1:4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" ht="30" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C29" s="3">
         <v>1262000</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" ht="75" spans="1:4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" ht="45" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C30" s="3">
         <v>111000</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C31" s="3">
         <v>2074000</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C32" s="3">
         <v>10000</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" ht="30" spans="1:4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C33" s="3">
         <v>4294350</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C34" s="3">
         <v>148093000</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C35" s="3">
         <v>165449000</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C36" s="3">
         <v>20000</v>
       </c>
       <c r="D36" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" ht="45" spans="1:4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" ht="30" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C37" s="3">
         <v>6331000</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" ht="30" spans="1:4">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C38" s="3">
         <v>90457200</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C39" s="3">
         <v>9725000</v>
       </c>
       <c r="D39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" ht="45" spans="1:4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" ht="30" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C40" s="3">
         <v>50000</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" ht="30" spans="1:4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C41" s="3">
         <v>165000</v>
       </c>
       <c r="D41" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" ht="75" spans="1:4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" ht="45" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C42" s="3">
         <v>120000</v>
       </c>
       <c r="D42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C43" s="3">
         <v>188359</v>
       </c>
       <c r="D43" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="44" ht="45" spans="1:4">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" ht="30" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C44" s="3">
         <v>87000</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="45" ht="30" spans="1:4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C45" s="3">
         <v>5866000</v>
       </c>
       <c r="D45" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="46" ht="30" spans="1:4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C46" s="3">
         <v>4839400</v>
       </c>
       <c r="D46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" ht="30" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C47" s="3">
         <v>506992</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="48" ht="30" spans="1:4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C48" s="3">
         <v>47850700</v>
       </c>
       <c r="D48" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" ht="30" spans="1:4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C49" s="3">
         <v>8260490</v>
       </c>
       <c r="D49" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C50" s="3">
         <v>31894000</v>
       </c>
       <c r="D50" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="51" ht="30" spans="1:4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C51" s="3">
         <v>1141000</v>
       </c>
       <c r="D51" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C52" s="3">
         <v>40454000</v>
       </c>
       <c r="D52" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C53" s="3">
         <v>100000</v>
       </c>
       <c r="D53" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="54" ht="45" spans="1:4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" ht="30" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C54" s="3">
         <v>1333000</v>
       </c>
       <c r="D54" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C55" s="3">
         <v>11000</v>
       </c>
       <c r="D55" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="56" ht="45" spans="1:4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" ht="30" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C56" s="3">
         <v>61612300</v>
@@ -3446,12 +3446,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" ht="45" spans="1:4">
+    <row r="57" ht="30" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C57" s="3">
         <v>309442000</v>
@@ -3462,58 +3462,58 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C58" s="3">
         <v>30884000</v>
       </c>
       <c r="D58" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C59" s="3">
         <v>226000</v>
       </c>
       <c r="D59" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C60" s="3">
         <v>11922000</v>
       </c>
       <c r="D60" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="61" ht="30" spans="1:4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C61" s="3">
         <v>13349000</v>
       </c>
       <c r="D61" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>